<commit_message>
Added scheduling of a crib with 4 workers to week10 of sed200.
</commit_message>
<xml_diff>
--- a/sed200/Week10/CribAssemblyComplete.xlsx
+++ b/sed200/Week10/CribAssemblyComplete.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel.watler\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seneca\MWATLER.github.io\sed200\Week10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Activity</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>The earliest we can finish is in 3.5 hours</t>
+  </si>
+  <si>
+    <t>What if we need a specialist for this, who is only available on Sundays?</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,6 +547,9 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">

</xml_diff>